<commit_message>
new version of dataLevel file
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/dataLevel.xlsx
+++ b/inbox-excel-vocabs/dataLevel.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/elter-vocabularies/work_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alessandrooggioni/Sites/GitHub/elter-vocabularies/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F86D7BAD-E180-D645-A75A-99BE180024DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F4382C-0F11-7942-A104-94454C1178A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" tabRatio="652" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16620" tabRatio="652" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" r:id="rId1"/>
@@ -1740,10 +1740,10 @@
     <t>level 4</t>
   </si>
   <si>
-    <t>eLTER_dl:06</t>
-  </si>
-  <si>
     <t>elter_dl:01, elter_dl:02, elter_dl:03, elter_dl:04, elter_dl:06</t>
+  </si>
+  <si>
+    <t>elter_dl:06</t>
   </si>
 </sst>
 </file>
@@ -7024,8 +7024,8 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -7175,9 +7175,9 @@
       </c>
       <c r="I6" s="23"/>
     </row>
-    <row r="7" spans="1:9" ht="48" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B7" s="23" t="s">
         <v>145</v>
@@ -7897,7 +7897,7 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
@@ -7943,7 +7943,7 @@
         <v>137</v>
       </c>
       <c r="D3" s="23" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E3" s="23" t="s">
         <v>138</v>

</xml_diff>